<commit_message>
R1: have 2 data dictionaries, FinalDataDictionary wich is from Rcodes, and FinalDataDictionaryWithDetails  has some more pieces of information about surveys
</commit_message>
<xml_diff>
--- a/Thesis/DataDictionary/FinalDataDictionaryWithDetails.xlsx
+++ b/Thesis/DataDictionary/FinalDataDictionaryWithDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sara ghasem pour\GitLab\Path2\Thesis\DataDictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8CE4C12-434B-4619-B373-772AA482E9C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13ACB017-F462-40F0-BF84-BF459FA2E19F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2306,8 +2306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J1016"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19705,8 +19705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F26" sqref="B26:F26"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20220,16 +20220,16 @@
         <v>615</v>
       </c>
       <c r="B26" s="5">
-        <v>1.3176470588235301</v>
+        <v>2.0409356725146202</v>
       </c>
       <c r="C26" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D26" s="5">
         <v>1</v>
       </c>
       <c r="E26" s="5">
-        <v>0.98162725310809995</v>
+        <v>0.96623420097394097</v>
       </c>
       <c r="F26" s="5">
         <v>172</v>

</xml_diff>

<commit_message>
R1: remove one of the question from Emotional questions ,becase it was instrumental question
</commit_message>
<xml_diff>
--- a/Thesis/DataDictionary/FinalDataDictionaryWithDetails.xlsx
+++ b/Thesis/DataDictionary/FinalDataDictionaryWithDetails.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sara ghasem pour\GitLab\Path2\Thesis\DataDictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55057D25-926D-434A-97CA-0E7AE3CBC8C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B975AE62-FF7B-47E2-9A0F-5734FC04A6BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BasicQuestions" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3372" uniqueCount="621">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3370" uniqueCount="620">
   <si>
     <t>Question</t>
   </si>
@@ -1763,9 +1763,6 @@
   </si>
   <si>
     <t>"I give my child something to eat to make him/her feel better when s/he is worried."</t>
-  </si>
-  <si>
-    <t>"I reward my child with something to eat when s/he is well behaved."</t>
   </si>
   <si>
     <t>"I give my child something to eat to make him/her feel better when s/he is feeling angry."</t>
@@ -2011,7 +2008,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -2020,6 +2017,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2318,8 +2316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J1017"/>
   <sheetViews>
-    <sheetView topLeftCell="A991" workbookViewId="0">
-      <selection activeCell="D1005" sqref="D1005"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2358,7 +2356,7 @@
         <v>553</v>
       </c>
       <c r="J1" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -2378,7 +2376,7 @@
         <v>3</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>552</v>
@@ -2390,7 +2388,7 @@
         <v>561</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -2422,7 +2420,7 @@
         <v>562</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -2442,7 +2440,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>556</v>
@@ -2451,7 +2449,7 @@
         <v>563</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -2480,7 +2478,7 @@
         <v>564</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -2509,7 +2507,7 @@
         <v>565</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -2538,7 +2536,7 @@
         <v>566</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -2563,9 +2561,6 @@
       <c r="H8" s="3" t="s">
         <v>560</v>
       </c>
-      <c r="I8" s="2" t="s">
-        <v>567</v>
-      </c>
       <c r="J8" s="1" t="s">
         <v>416</v>
       </c>
@@ -2590,7 +2585,7 @@
         <v>69</v>
       </c>
       <c r="H9" s="3"/>
-      <c r="I9" s="2"/>
+      <c r="I9" s="8"/>
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -2714,10 +2709,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -3785,7 +3780,7 @@
         <v>97</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D80" s="4">
         <v>1</v>
@@ -3819,7 +3814,7 @@
         <v>97</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="D82" s="4">
         <v>2</v>
@@ -3836,7 +3831,7 @@
         <v>97</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D83" s="4">
         <v>1</v>
@@ -3870,7 +3865,7 @@
         <v>97</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D85" s="4">
         <v>1</v>
@@ -3921,7 +3916,7 @@
         <v>97</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D88" s="4">
         <v>1</v>
@@ -3989,7 +3984,7 @@
         <v>97</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D92" s="4">
         <v>1</v>
@@ -4006,7 +4001,7 @@
         <v>97</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D93" s="4">
         <v>1</v>
@@ -4074,7 +4069,7 @@
         <v>97</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D97" s="4">
         <v>1</v>
@@ -4125,7 +4120,7 @@
         <v>97</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="D100" s="4">
         <v>4</v>
@@ -4159,7 +4154,7 @@
         <v>97</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="D102" s="4">
         <v>1</v>
@@ -4176,7 +4171,7 @@
         <v>97</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D103" s="4">
         <v>2</v>
@@ -4210,7 +4205,7 @@
         <v>97</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D105" s="4">
         <v>1</v>
@@ -4295,7 +4290,7 @@
         <v>97</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="D110" s="4">
         <v>1</v>
@@ -4312,7 +4307,7 @@
         <v>97</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="D111" s="4">
         <v>1</v>
@@ -4346,7 +4341,7 @@
         <v>97</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D113" s="4">
         <v>1</v>
@@ -4380,7 +4375,7 @@
         <v>97</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="D115" s="4">
         <v>1</v>
@@ -4431,7 +4426,7 @@
         <v>97</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="D118" s="4">
         <v>1</v>
@@ -4516,7 +4511,7 @@
         <v>97</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D123" s="4">
         <v>1</v>
@@ -4533,7 +4528,7 @@
         <v>97</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="D124" s="4">
         <v>1</v>
@@ -4550,7 +4545,7 @@
         <v>97</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="D125" s="4">
         <v>1</v>
@@ -4584,7 +4579,7 @@
         <v>97</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="D127" s="4">
         <v>1</v>
@@ -4669,7 +4664,7 @@
         <v>97</v>
       </c>
       <c r="C132" s="4" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D132" s="4">
         <v>1</v>
@@ -4737,7 +4732,7 @@
         <v>97</v>
       </c>
       <c r="C136" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D136" s="4">
         <v>1</v>
@@ -4754,7 +4749,7 @@
         <v>97</v>
       </c>
       <c r="C137" s="4" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="D137" s="4">
         <v>1</v>
@@ -4771,7 +4766,7 @@
         <v>97</v>
       </c>
       <c r="C138" s="4" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="D138" s="4">
         <v>1</v>
@@ -4788,7 +4783,7 @@
         <v>97</v>
       </c>
       <c r="C139" s="4" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="D139" s="4">
         <v>1</v>
@@ -4822,7 +4817,7 @@
         <v>97</v>
       </c>
       <c r="C141" s="4" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="D141" s="4">
         <v>1</v>
@@ -4839,7 +4834,7 @@
         <v>97</v>
       </c>
       <c r="C142" s="4" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="D142" s="4">
         <v>1</v>
@@ -5009,7 +5004,7 @@
         <v>97</v>
       </c>
       <c r="C152" s="4" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="D152" s="4">
         <v>1</v>
@@ -5060,7 +5055,7 @@
         <v>97</v>
       </c>
       <c r="C155" s="4" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="D155" s="4">
         <v>1</v>
@@ -5145,7 +5140,7 @@
         <v>97</v>
       </c>
       <c r="C160" s="4" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="D160" s="4">
         <v>1</v>
@@ -5162,7 +5157,7 @@
         <v>97</v>
       </c>
       <c r="C161" s="4" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="D161" s="4">
         <v>1</v>
@@ -5230,7 +5225,7 @@
         <v>97</v>
       </c>
       <c r="C165" s="4" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="D165" s="4">
         <v>1</v>
@@ -5247,7 +5242,7 @@
         <v>97</v>
       </c>
       <c r="C166" s="4" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="D166" s="4">
         <v>1</v>
@@ -19212,87 +19207,87 @@
       </c>
     </row>
     <row r="988" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A988" s="2" t="s">
+      <c r="A988" s="8" t="s">
         <v>483</v>
       </c>
-      <c r="B988" s="2" t="s">
+      <c r="B988" s="8" t="s">
         <v>484</v>
       </c>
-      <c r="C988" s="2" t="s">
+      <c r="C988" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="D988" s="2">
+      <c r="D988" s="8">
         <v>75</v>
       </c>
-      <c r="E988" s="2">
+      <c r="E988" s="8">
         <v>3</v>
       </c>
     </row>
     <row r="989" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A989" s="2" t="s">
+      <c r="A989" s="8" t="s">
         <v>483</v>
       </c>
-      <c r="B989" s="2" t="s">
+      <c r="B989" s="8" t="s">
         <v>484</v>
       </c>
-      <c r="C989" s="2" t="s">
+      <c r="C989" s="8" t="s">
         <v>369</v>
       </c>
-      <c r="D989" s="2">
+      <c r="D989" s="8">
         <v>33</v>
       </c>
-      <c r="E989" s="2">
+      <c r="E989" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="990" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A990" s="2" t="s">
+      <c r="A990" s="8" t="s">
         <v>483</v>
       </c>
-      <c r="B990" s="2" t="s">
+      <c r="B990" s="8" t="s">
         <v>484</v>
       </c>
-      <c r="C990" s="2" t="s">
+      <c r="C990" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="D990" s="2">
+      <c r="D990" s="8">
         <v>35</v>
       </c>
-      <c r="E990" s="2">
+      <c r="E990" s="8">
         <v>4</v>
       </c>
     </row>
     <row r="991" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A991" s="2" t="s">
+      <c r="A991" s="8" t="s">
         <v>483</v>
       </c>
-      <c r="B991" s="2" t="s">
+      <c r="B991" s="8" t="s">
         <v>484</v>
       </c>
-      <c r="C991" s="2" t="s">
+      <c r="C991" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="D991" s="2">
+      <c r="D991" s="8">
         <v>14</v>
       </c>
-      <c r="E991" s="2">
+      <c r="E991" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="992" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A992" s="2" t="s">
+      <c r="A992" s="8" t="s">
         <v>483</v>
       </c>
-      <c r="B992" s="2" t="s">
+      <c r="B992" s="8" t="s">
         <v>484</v>
       </c>
-      <c r="C992" s="2" t="s">
+      <c r="C992" s="8" t="s">
         <v>370</v>
       </c>
-      <c r="D992" s="2">
+      <c r="D992" s="8">
         <v>16</v>
       </c>
-      <c r="E992" s="2">
+      <c r="E992" s="8">
         <v>5</v>
       </c>
     </row>
@@ -19731,10 +19726,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23:F29"/>
+      <selection activeCell="A20" sqref="A20:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19761,7 +19756,7 @@
         <v>498</v>
       </c>
       <c r="F1" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -19926,19 +19921,19 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>483</v>
+        <v>469</v>
       </c>
       <c r="B10" s="2">
-        <v>3.0465116279069799</v>
+        <v>2.3720930232558102</v>
       </c>
       <c r="C10" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D10" s="2">
         <v>1</v>
       </c>
       <c r="E10" s="2">
-        <v>1.03626608996952</v>
+        <v>1.28914960526169</v>
       </c>
       <c r="F10" s="2">
         <v>173</v>
@@ -19946,10 +19941,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="B11" s="2">
-        <v>2.3720930232558102</v>
+        <v>2.56395348837209</v>
       </c>
       <c r="C11" s="2">
         <v>2</v>
@@ -19958,7 +19953,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="2">
-        <v>1.28914960526169</v>
+        <v>1.20500057418614</v>
       </c>
       <c r="F11" s="2">
         <v>173</v>
@@ -19966,50 +19961,50 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>465</v>
+        <v>443</v>
       </c>
       <c r="B12" s="2">
-        <v>2.56395348837209</v>
+        <v>2.86046511627907</v>
       </c>
       <c r="C12" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D12" s="2">
         <v>1</v>
       </c>
       <c r="E12" s="2">
-        <v>1.20500057418614</v>
+        <v>1.2580760461742</v>
       </c>
       <c r="F12" s="2">
         <v>173</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>443</v>
-      </c>
-      <c r="B13" s="2">
-        <v>2.86046511627907</v>
-      </c>
-      <c r="C13" s="2">
+      <c r="A13" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="B13" s="1">
+        <v>3.1046511627907001</v>
+      </c>
+      <c r="C13" s="1">
         <v>3</v>
       </c>
-      <c r="D13" s="2">
-        <v>1</v>
-      </c>
-      <c r="E13" s="2">
-        <v>1.2580760461742</v>
-      </c>
-      <c r="F13" s="2">
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.98561667420867605</v>
+      </c>
+      <c r="F13" s="1">
         <v>173</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>431</v>
+        <v>415</v>
       </c>
       <c r="B14" s="1">
-        <v>3.1046511627907001</v>
+        <v>3.0467836257309902</v>
       </c>
       <c r="C14" s="1">
         <v>3</v>
@@ -20018,7 +20013,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="1">
-        <v>0.98561667420867605</v>
+        <v>1.03930330452141</v>
       </c>
       <c r="F14" s="1">
         <v>173</v>
@@ -20026,19 +20021,19 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>415</v>
+        <v>399</v>
       </c>
       <c r="B15" s="1">
-        <v>3.0467836257309902</v>
+        <v>3.6220930232558102</v>
       </c>
       <c r="C15" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D15" s="1">
         <v>1</v>
       </c>
       <c r="E15" s="1">
-        <v>1.03930330452141</v>
+        <v>1.04415960362666</v>
       </c>
       <c r="F15" s="1">
         <v>173</v>
@@ -20046,19 +20041,19 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>399</v>
+        <v>387</v>
       </c>
       <c r="B16" s="1">
-        <v>3.6220930232558102</v>
+        <v>3.2209302325581399</v>
       </c>
       <c r="C16" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D16" s="1">
         <v>1</v>
       </c>
       <c r="E16" s="1">
-        <v>1.04415960362666</v>
+        <v>1.0362004682052199</v>
       </c>
       <c r="F16" s="1">
         <v>173</v>
@@ -20066,10 +20061,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="B17" s="1">
-        <v>3.2209302325581399</v>
+        <v>3.17441860465116</v>
       </c>
       <c r="C17" s="1">
         <v>3</v>
@@ -20078,109 +20073,109 @@
         <v>1</v>
       </c>
       <c r="E17" s="1">
-        <v>1.0362004682052199</v>
+        <v>1.0889327407162901</v>
       </c>
       <c r="F17" s="1">
         <v>173</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="B18" s="1">
-        <v>3.17441860465116</v>
-      </c>
-      <c r="C18" s="1">
+      <c r="A18" s="5" t="s">
+        <v>499</v>
+      </c>
+      <c r="B18" s="5">
+        <v>3.2267441860465098</v>
+      </c>
+      <c r="C18" s="5">
         <v>3</v>
       </c>
-      <c r="D18" s="1">
-        <v>1</v>
-      </c>
-      <c r="E18" s="1">
-        <v>1.0889327407162901</v>
-      </c>
-      <c r="F18" s="1">
+      <c r="D18" s="5">
+        <v>3</v>
+      </c>
+      <c r="E18" s="5">
+        <v>0.41994831723354598</v>
+      </c>
+      <c r="F18" s="5">
         <v>173</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
-        <v>499</v>
-      </c>
-      <c r="B19" s="5">
-        <v>3.2267441860465098</v>
-      </c>
-      <c r="C19" s="5">
-        <v>3</v>
-      </c>
-      <c r="D19" s="5">
-        <v>3</v>
-      </c>
-      <c r="E19" s="5">
-        <v>0.41994831723354598</v>
-      </c>
-      <c r="F19" s="5">
+      <c r="A19" s="7" t="s">
+        <v>500</v>
+      </c>
+      <c r="B19" s="7">
+        <v>3.0672128259337601</v>
+      </c>
+      <c r="C19" s="7">
+        <v>2.9583333333333299</v>
+      </c>
+      <c r="D19" s="7">
+        <v>1.75</v>
+      </c>
+      <c r="E19" s="7">
+        <v>0.67160753514376603</v>
+      </c>
+      <c r="F19" s="7">
         <v>173</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="7" t="s">
-        <v>500</v>
-      </c>
-      <c r="B20" s="7">
-        <v>3.0672128259337601</v>
-      </c>
-      <c r="C20" s="7">
-        <v>2.9583333333333299</v>
-      </c>
-      <c r="D20" s="7">
-        <v>1.75</v>
-      </c>
-      <c r="E20" s="7">
-        <v>0.67160753514376603</v>
-      </c>
-      <c r="F20" s="7">
+      <c r="A20" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="B20" s="2">
+        <v>3.0690274841437599</v>
+      </c>
+      <c r="C20" s="2">
+        <v>2.9090909090909101</v>
+      </c>
+      <c r="D20" s="2">
+        <v>1.7272730000000001</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0.67234047518751605</v>
+      </c>
+      <c r="F20" s="2">
         <v>173</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>501</v>
-      </c>
-      <c r="B21" s="2">
-        <v>3.0672128259337601</v>
-      </c>
-      <c r="C21" s="2">
-        <v>2.9583333333333299</v>
-      </c>
-      <c r="D21" s="2">
-        <v>1.75</v>
-      </c>
-      <c r="E21" s="2">
-        <v>0.67160753514376603</v>
-      </c>
-      <c r="F21" s="2">
+      <c r="A21" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="B21" s="1">
+        <v>3.2340116279069799</v>
+      </c>
+      <c r="C21" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="D21" s="1">
+        <v>2</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0.54549474285632105</v>
+      </c>
+      <c r="F21" s="1">
         <v>173</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>502</v>
-      </c>
-      <c r="B22" s="1">
-        <v>3.2340116279069799</v>
-      </c>
-      <c r="C22" s="1">
-        <v>3.2</v>
-      </c>
-      <c r="D22" s="1">
-        <v>2</v>
-      </c>
-      <c r="E22" s="1">
-        <v>0.54549474285632105</v>
-      </c>
-      <c r="F22" s="1">
+      <c r="A22" s="5" t="s">
+        <v>576</v>
+      </c>
+      <c r="B22" s="5">
+        <v>4.4011627906976702</v>
+      </c>
+      <c r="C22" s="5">
+        <v>4</v>
+      </c>
+      <c r="D22" s="5">
+        <v>1</v>
+      </c>
+      <c r="E22" s="5">
+        <v>1.46961380024897</v>
+      </c>
+      <c r="F22" s="5">
         <v>173</v>
       </c>
     </row>
@@ -20189,7 +20184,7 @@
         <v>577</v>
       </c>
       <c r="B23" s="5">
-        <v>4.4011627906976702</v>
+        <v>3.8947368421052602</v>
       </c>
       <c r="C23" s="5">
         <v>4</v>
@@ -20198,7 +20193,7 @@
         <v>1</v>
       </c>
       <c r="E23" s="5">
-        <v>1.46961380024897</v>
+        <v>1.0292923415911599</v>
       </c>
       <c r="F23" s="5">
         <v>173</v>
@@ -20206,19 +20201,19 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="B24" s="5">
-        <v>3.8947368421052602</v>
-      </c>
-      <c r="C24" s="5">
-        <v>4</v>
+        <v>4.2441860465116301</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>619</v>
       </c>
       <c r="D24" s="5">
         <v>1</v>
       </c>
       <c r="E24" s="5">
-        <v>1.0292923415911599</v>
+        <v>1.09689670185529</v>
       </c>
       <c r="F24" s="5">
         <v>173</v>
@@ -20229,16 +20224,14 @@
         <v>581</v>
       </c>
       <c r="B25" s="5">
-        <v>4.2441860465116301</v>
+        <v>2.0409356725146202</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>620</v>
-      </c>
-      <c r="D25" s="5">
-        <v>1</v>
-      </c>
+        <v>619</v>
+      </c>
+      <c r="D25" s="5"/>
       <c r="E25" s="5">
-        <v>1.09689670185529</v>
+        <v>0.96623420097394097</v>
       </c>
       <c r="F25" s="5">
         <v>173</v>
@@ -20249,14 +20242,16 @@
         <v>582</v>
       </c>
       <c r="B26" s="5">
-        <v>2.0409356725146202</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>620</v>
-      </c>
-      <c r="D26" s="5"/>
+        <v>1.31395348837209</v>
+      </c>
+      <c r="C26" s="5">
+        <v>1</v>
+      </c>
+      <c r="D26" s="5">
+        <v>1</v>
+      </c>
       <c r="E26" s="5">
-        <v>0.96623420097394097</v>
+        <v>0.97646729187055903</v>
       </c>
       <c r="F26" s="5">
         <v>173</v>
@@ -20267,16 +20262,16 @@
         <v>583</v>
       </c>
       <c r="B27" s="5">
-        <v>1.31395348837209</v>
+        <v>1.7674418604651201</v>
       </c>
       <c r="C27" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D27" s="5">
         <v>1</v>
       </c>
       <c r="E27" s="5">
-        <v>0.97646729187055903</v>
+        <v>0.437280768253347</v>
       </c>
       <c r="F27" s="5">
         <v>173</v>
@@ -20287,38 +20282,18 @@
         <v>584</v>
       </c>
       <c r="B28" s="5">
-        <v>1.7674418604651201</v>
+        <v>1.44767441860465</v>
       </c>
       <c r="C28" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D28" s="5">
         <v>1</v>
       </c>
       <c r="E28" s="5">
-        <v>0.437280768253347</v>
+        <v>0.498706336771368</v>
       </c>
       <c r="F28" s="5">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="5" t="s">
-        <v>585</v>
-      </c>
-      <c r="B29" s="5">
-        <v>1.44767441860465</v>
-      </c>
-      <c r="C29" s="5">
-        <v>1</v>
-      </c>
-      <c r="D29" s="5">
-        <v>1</v>
-      </c>
-      <c r="E29" s="5">
-        <v>0.498706336771368</v>
-      </c>
-      <c r="F29" s="5">
         <v>173</v>
       </c>
     </row>

</xml_diff>